<commit_message>
Sub-tests with page objects
</commit_message>
<xml_diff>
--- a/Selectors2ObjectRepository/LIS_Login/Main.rvl.xlsx
+++ b/Selectors2ObjectRepository/LIS_Login/Main.rvl.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="40">
   <si>
     <t>Flow</t>
   </si>
@@ -103,6 +103,36 @@
   </si>
   <si>
     <t>LogOut</t>
+  </si>
+  <si>
+    <t>DoPlayTest</t>
+  </si>
+  <si>
+    <t>sstestPath</t>
+  </si>
+  <si>
+    <t>%WORKDIR%\PO_Home\PO_Home.sstest</t>
+  </si>
+  <si>
+    <t>sheetName</t>
+  </si>
+  <si>
+    <t>Param</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>DoPlayScript</t>
+  </si>
+  <si>
+    <t>scriptPath</t>
+  </si>
+  <si>
+    <t>%WORKDIR%\Main.rvl.xlsx</t>
+  </si>
+  <si>
+    <t>%WORKDIR%\PO_Login\PO_Login.sstest</t>
   </si>
 </sst>
 </file>
@@ -123,7 +153,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="163">
+  <borders count="170">
     <border>
       <left/>
       <right/>
@@ -293,11 +323,18 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
@@ -461,6 +498,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="160" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="161" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="162" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="163" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="164" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="165" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="166" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="167" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="168" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="169" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,7 +514,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H17"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.5546875" customWidth="true"/>
@@ -563,224 +607,166 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="33"/>
-      <c r="B5" s="34" t="s">
+      <c r="A5" s="89"/>
+      <c r="B5" s="90"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="95"/>
+      <c r="H5" s="96"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="97"/>
+      <c r="B6" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="40"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="41"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="48"/>
+      <c r="C6" s="99" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="100" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="101" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="102" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="103" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="104"/>
     </row>
     <row r="7">
-      <c r="A7" s="49"/>
-      <c r="B7" s="50" t="s">
+      <c r="A7" s="105"/>
+      <c r="B7" s="106" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="107"/>
+      <c r="D7" s="108"/>
+      <c r="E7" s="109" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="110" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="111" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="112"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="113"/>
+      <c r="B8" s="114"/>
+      <c r="C8" s="115"/>
+      <c r="D8" s="116"/>
+      <c r="E8" s="117"/>
+      <c r="F8" s="118"/>
+      <c r="G8" s="119"/>
+      <c r="H8" s="120"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="121"/>
+      <c r="B9" s="122" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="51" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="54" t="s">
+      <c r="C9" s="123" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="124" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="125" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="126" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="55" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="56"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="57"/>
-      <c r="B8" s="58" t="s">
+      <c r="G9" s="127" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="128"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="129"/>
+      <c r="B10" s="130" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="131"/>
+      <c r="D10" s="132"/>
+      <c r="E10" s="133" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="134" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="135" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="136"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="137"/>
+      <c r="B11" s="138"/>
+      <c r="C11" s="139"/>
+      <c r="D11" s="140"/>
+      <c r="E11" s="141"/>
+      <c r="F11" s="142"/>
+      <c r="G11" s="143"/>
+      <c r="H11" s="144"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="145"/>
+      <c r="B12" s="146" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="59" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="61" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="62" t="s">
+      <c r="C12" s="147" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="148" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="149" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="150" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="63" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="64"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="65"/>
-      <c r="B9" s="66" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="67" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="68" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="69" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="71" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="72"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="73"/>
-      <c r="B10" s="74"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="77"/>
-      <c r="F10" s="78"/>
-      <c r="G10" s="79"/>
-      <c r="H10" s="80"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="81"/>
-      <c r="B11" s="82" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="83" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="84" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="85" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="86" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" s="87" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" s="88"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="89"/>
-      <c r="B12" s="90"/>
-      <c r="C12" s="91"/>
-      <c r="D12" s="92"/>
-      <c r="E12" s="93"/>
-      <c r="F12" s="94"/>
-      <c r="G12" s="95"/>
-      <c r="H12" s="96"/>
+      <c r="G12" s="151" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="152"/>
     </row>
     <row r="13">
-      <c r="A13" s="97"/>
-      <c r="B13" s="98"/>
-      <c r="C13" s="99"/>
-      <c r="D13" s="100"/>
-      <c r="E13" s="101"/>
-      <c r="F13" s="102"/>
-      <c r="G13" s="103"/>
-      <c r="H13" s="104"/>
+      <c r="A13" s="153"/>
+      <c r="B13" s="154" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="155"/>
+      <c r="D13" s="156"/>
+      <c r="E13" s="157" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="158" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="159" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="160"/>
     </row>
     <row r="14">
-      <c r="A14" s="105"/>
-      <c r="B14" s="106"/>
-      <c r="C14" s="107"/>
-      <c r="D14" s="108"/>
-      <c r="E14" s="109"/>
-      <c r="F14" s="110"/>
-      <c r="G14" s="111"/>
-      <c r="H14" s="112"/>
+      <c r="A14" s="164"/>
     </row>
     <row r="15">
-      <c r="A15" s="113"/>
-      <c r="B15" s="114"/>
-      <c r="C15" s="115"/>
-      <c r="D15" s="116"/>
-      <c r="E15" s="117"/>
-      <c r="F15" s="118"/>
-      <c r="G15" s="119"/>
-      <c r="H15" s="120"/>
+      <c r="A15" s="166"/>
     </row>
     <row r="16">
-      <c r="A16" s="121"/>
-      <c r="B16" s="122"/>
-      <c r="C16" s="123"/>
-      <c r="D16" s="124"/>
-      <c r="E16" s="125"/>
-      <c r="F16" s="126"/>
-      <c r="G16" s="127"/>
-      <c r="H16" s="128"/>
+      <c r="A16" s="167"/>
     </row>
     <row r="17">
-      <c r="A17" s="129"/>
-      <c r="B17" s="130"/>
-      <c r="C17" s="131"/>
-      <c r="D17" s="132"/>
-      <c r="E17" s="133"/>
-      <c r="F17" s="134"/>
-      <c r="G17" s="135"/>
-      <c r="H17" s="136"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="137"/>
-      <c r="B18" s="138"/>
-      <c r="C18" s="139"/>
-      <c r="D18" s="140"/>
-      <c r="E18" s="141"/>
-      <c r="F18" s="142"/>
-      <c r="G18" s="143"/>
-      <c r="H18" s="144"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="145"/>
-      <c r="B19" s="146"/>
-      <c r="C19" s="147"/>
-      <c r="D19" s="148"/>
-      <c r="E19" s="149"/>
-      <c r="F19" s="150"/>
-      <c r="G19" s="151"/>
-      <c r="H19" s="152"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="153"/>
-      <c r="B20" s="154"/>
-      <c r="C20" s="155"/>
-      <c r="D20" s="156"/>
-      <c r="E20" s="157"/>
-      <c r="F20" s="158"/>
-      <c r="G20" s="159"/>
-      <c r="H20" s="160"/>
+      <c r="A17" s="168"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>